<commit_message>
add in ie fallback
</commit_message>
<xml_diff>
--- a/js/data2.xlsx
+++ b/js/data2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18580" yWindow="6760" windowWidth="18220" windowHeight="15280" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="data.csv" sheetId="1" r:id="rId1"/>
@@ -192,35 +192,6 @@
     <t>a,b,c,e,f</t>
   </si>
   <si>
-    <r>
-      <t>Hydropower provides more than 70% of the Northwest's electricity and is an important export to California and Canada (EIA 2014a, EIA 2014b). Warmer temperatures and less mountain snowpack will shift peak streamflow in the region from summer toward spring (BPA 2011, CIG 2009, DOE 2012, Doppelt 2009, USGCRP 2014). Meanwhile, warmer temperatures will likely increase electricity demand for cooling in the summer, when available hydropower generation is reduced (BPA 2011, DOE 2012, DOE 2013, USGCRP 2014). Warmer and drier summers may also increase the threat of wildfires, which have the potential to disrupt electricity transmission (DOE 2013, USGCRP 2014).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF4F81BD"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t>Many energy systems in the Southwest are already designed for hot and arid conditions, but system reliability is increasingly threatened by higher temperatures, declining water availability, and greater risk of wildfire (DOE 2013, NOAA 2013, USGCRP 2014). More frequent and severe heat waves are likely to amplify demand for cooling energy (NOAA 2013, Sathaye et al. 2012, USGCRP 2014). Higher temperatures and reduced water availability may limit the ability of natural gas-fired, coal-fired, and other thermoelectric power plants in the region to meet demand (DOE 2013, Sathaye et al. 2012). Hydropower resources will be affected by reductions in streamflow and shifts in streamflow timing (AEG and Cubed 2005, Cayan et al. 2013, NOAA 2013, USGCRP 2014). Electricity transmission lines essential to connecting remote generation assets to demand centers are vulnerable to projected increases in wildfire as forests and shrub lands become drier (DOE 2013, Sathaye et al. 2012, USGCRP 2014).</t>
-  </si>
-  <si>
-    <t>The Northern Great Plains produces coal, crude oil, and biofuel for use across the nation (EIA 2012, EIA 2014c). Delivery is mainly by railroad and pipeline, which are vulnerable to damage or disruption from increasing heavy precipitation events and associated flooding and erosion (USGCRP 2014). Summer heat waves could also damage railroad tracks and are likely to reduce thermoelectric power plant and transmission line capacity (DOE 2013, USGCRP 2014). Higher temperatures could lower the yields of crops used for biofuels while expanding northward the range in which certain biofuel crops (e.g., corn) can be cultivated (NOAA 2013, Roberts and Schlenker 2011, USGCRP 2014).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Southern Great Plains is home to substantial oil and gas production, refining, and transportation assets, with an especially high concentration near the Gulf Coast. Projected increases in the intensity of Atlantic hurricanes and associated rainfall, combined with rising global sea levels and subsiding coastlines, escalate the risk of coastal flooding and wind damage to many of these assets (DOE 2013, USGCRP 2014, DOE 2015). Heat waves and higher temperatures are also projected for the region, increasing electricity demand for cooling while reducing the generation capacity of thermoelectric power plants and the transmission capacity of power lines (DOE 2013, NOAA 2013, USGCRP 2014). Drought and increased competition for water could limit the water available for power plant cooling and oil and gas operations (Cook et al. 2013, DOE 2013, USGCRP 2014). </t>
-  </si>
-  <si>
-    <t>More than 90% of the region’s electricity is generated by coal-fired and other thermoelectric power plants, which are vulnerable to increasing temperatures (DOE 2013, EIA 2013). Warmer temperatures reduce the generation capacity of power plants and the transmission capacity of power lines, while simultaneously increasing electricity demand for cooling (DOE 2013, USGCRP 2014). Energy-related infrastructure, including roads, railroads, and electric grid equipment, may also be at increased risk of damage due to flooding, as heavy precipitation events are projected to occur more frequently (DOE 2013, NOAA 2013, USGCRP 2014). Increased risk of floods and droughts may disrupt fuel transport on inlands waterways. Changing water availability and increasing temperatures may also affect biofuel production and refining capacity in the Midwest (NOAA 2013, USGCRP 2014).</t>
-  </si>
-  <si>
-    <t>The Northeast region is comparatively cool, so as temperatures rise, increased electricity demand for cooling is likely to be driven in part by increasing market penetration of air conditioners (Auffhammer 2011, DOE 2013, NOAA 2013, USGCRP 2014). Warmer temperatures and more intense heat waves also reduce the capacity of thermoelectric power plants and electric grid transmission during periods of peak electricity demand (DOE 2013, USGCRP 2014). Sea level rise and storm surge increasingly threaten coastal energy infrastructure, including ports, electric grid equipment, and power plants (DOE 2013, USGCRP 2014). Farther inland, low-lying infrastructure, such as roads, railroads, refineries, and power lines, is vulnerable to more frequent flooding from heavy precipitation events (DOE 2013, NOAA 2013, USGCRP 2014).</t>
-  </si>
-  <si>
     <t xml:space="preserve">The Southeast, especially the northern Gulf Coast, hosts a large amount of energy infrastructure in low-lying coastal plains that are vulnerable to increases in flooding (DOE 2013, USGCRP 2014). High winds, coastal erosion, flooding, and large waves from hurricanes and sea level rise-enhanced storm surge threaten oil and gas production, ports, pipelines, refineries, and storage facilities, as well as electricity generation and transmission assets (DOE 2013, USGCRP 2014, DOE 2015). Higher temperatures and more frequent, severe, and longer-lasting heat waves are also projected for the Southeast, potentially increasing peak electricity demand for cooling while reducing the capacity of the thermoelectric generation and transmission systems needed to meet the increased demand (DOE 2013, NOAA 2013, USGCRP 2014). </t>
   </si>
   <si>
@@ -228,6 +199,24 @@
   </si>
   <si>
     <t>Hawaii and Puerto Rico share many similarities in their energy systems, including reliance on imported petroleum and other fuels. In both of the island regions, projected sea level rise and hurricane-driven storm surge threaten ports and other essential coastal energy infrastructure with flooding, wave damage, and erosion, while hurricane winds pose a danger to structures and power lines (DOE 2013, Murakami et al. 2013, PRCCC 2013, USGCRP 2014). Higher temperatures reduce the efficiency of oil-fired and other thermoelectric power plants, significantly restricting electricity supply if such losses are not offset by reduced demand or supplies added elsewhere in the system (DOE 2013). Other U.S. islands in the Pacific and in the Caribbean are not separately examined in this report but are likely to have similar climate impacts and resilience solutions as Hawaii and Puerto Rico.</t>
+  </si>
+  <si>
+    <t>Hydropower is a major source of electricity in the Northwest, providing more than 70% of the region’s power. Warmer temperatures and less mountain snowpack will cause streams fed by melting snow to reach their peak flow earlier in spring, leading to less available hydropower during the hot summer months when demand is highest. Increased wildfire threat also has the potential to disrupt electricity transmission.</t>
+  </si>
+  <si>
+    <t>Many energy systems in the Southwest are already designed for hot and arid conditions, but climate change is going to put additional pressure on the region. More frequent and severe heat waves will drive up electricity demand as people try to stay cool, while at the same time hampering the ability of natural gas- and coal-fired power plants to meet that demand. Other concerns as the region becomes drier include decreasing hydropower resources and wildfires threatening transmission lines.</t>
+  </si>
+  <si>
+    <t>The Northern Great Plains produces coal, crude oil and biofuel for use across the nation. Delivery is mainly by railroad and pipeline, which are vulnerable to the increasing heavy rains and extreme heat associated with climate change. Heat waves can also reduce the capacity of natural gas and coal power plants, in addition to lowering the yields of crops used for biofuels.</t>
+  </si>
+  <si>
+    <t>The Southern Great Plains is home to oil and gas production, refining and transportation, with an especially high concentration near the Gulf Coast. The growing threat from Atlantic hurricanes and sea level rise puts that important energy resource at risk from coastal flooding and wind damage. Heat waves and drought are also a concern in this region, increasing electricity demand and reducing the generation capacity of many types of power plants.</t>
+  </si>
+  <si>
+    <t>More than 90% of the Midwest’s electricity is generated by coal-fired and other thermoelectric power plants. High temperatures can reduce both the generation capacity of those plants and the transmission capacity of power lines, while simultaneously increasing electricity demand for cooling. Drought and flooding can further disrupt fuel transport over land and water, in addition to hurting biofuel production and refining capacity in the region.</t>
+  </si>
+  <si>
+    <t>The Northeast region is comparatively cool, so as temperatures rise, increasing use of air conditioners is likely to drive up electricity demand. Hotter temperatures can also reduce the capacity of power plants and electric grid transmission during periods of high demand. Along the coast, sea level rise and storm surge can threaten ports, electric grid equipment and power plants, while flooding from heavy rains can endanger energy infrastructure further inland such as roads, railroads, refineries and power lines.</t>
   </si>
 </sst>
 </file>
@@ -265,10 +254,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF4F81BD"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
     </font>
   </fonts>
   <fills count="2">
@@ -305,10 +293,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -658,19 +649,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -728,7 +720,7 @@
         <v>40</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -751,7 +743,7 @@
         <v>34</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -776,8 +768,8 @@
       <c r="I4" t="s">
         <v>46</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>57</v>
+      <c r="L4" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -805,8 +797,8 @@
       <c r="I5" t="s">
         <v>49</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>58</v>
+      <c r="L5" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -837,8 +829,8 @@
       <c r="K6" t="s">
         <v>43</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>59</v>
+      <c r="L6" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -863,8 +855,8 @@
       <c r="I7" t="s">
         <v>53</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>60</v>
+      <c r="L7" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -889,8 +881,8 @@
       <c r="K8" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>61</v>
+      <c r="L8" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -919,7 +911,7 @@
         <v>53</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -941,8 +933,8 @@
       <c r="I10" t="s">
         <v>56</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>62</v>
+      <c r="L10" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:12">

</xml_diff>